<commit_message>
Internationalize stream search UI strings and compute placeholder hours
- Introduce `num_hours` for placeholder calculation.
- Replace hard‑coded placeholder with `LanguageTranslator.translate("stream_search_phrase")`, inserting `{num_hours}`.
- Localize short‑query warning, spinner text, and connection‑error info via `LanguageTranslator.translate`.
</commit_message>
<xml_diff>
--- a/streamlit_ui/resources/language/ui_lang_def.xlsx
+++ b/streamlit_ui/resources/language/ui_lang_def.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="670">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="683">
   <si>
     <t xml:space="preserve">code_name</t>
   </si>
@@ -2401,6 +2401,45 @@
   <si>
     <t xml:space="preserve">very simple language</t>
   </si>
+  <si>
+    <t xml:space="preserve">stream_search_phrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ui_utils_public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wybierz lub podaj frazę do wyszukania w wybranych stronach (ostatnie {num_hours}h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select or enter a phrase to search in the chosen pages (last {num_hours}h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stream_search_to_short_phrase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zapytanie musi posiadać co majmniej {MIN_STREAM_QUERY_LEN} znaków</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The query must contain at least {MIN_STREAM_QUERY_LEN} characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stream_searching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyszukiwanie…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Searching…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stream_searching_problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem z poiłączeniem, spróbuj jeszcze raz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connection problem, please try again</t>
+  </si>
 </sst>
 </file>
 
@@ -2409,7 +2448,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2470,6 +2509,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2522,7 +2567,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2593,6 +2638,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2673,10 +2722,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H210"/>
+  <dimension ref="A1:H214"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D159" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F210" activeCellId="0" sqref="F210"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A192" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B213" activeCellId="0" sqref="B213:C214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6789,6 +6838,86 @@
       </c>
       <c r="F210" s="0" t="s">
         <v>669</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D211" s="1" t="n">
+        <v>901</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="F211" s="0" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="18" t="s">
+        <v>674</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D212" s="1" t="n">
+        <v>913</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="F212" s="0" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A213" s="18" t="s">
+        <v>677</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D213" s="1" t="n">
+        <v>918</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="F213" s="0" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A214" s="18" t="s">
+        <v>680</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D214" s="1" t="n">
+        <v>931</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="F214" s="0" t="s">
+        <v>682</v>
       </c>
     </row>
   </sheetData>

</xml_diff>